<commit_message>
fix bug kwr004 #118535
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR004_v2.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR004_v2.xlsx
@@ -136,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -249,6 +249,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -256,7 +356,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment shrinkToFit="1"/>
@@ -301,30 +401,26 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -338,6 +434,55 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,7 +869,7 @@
   <sheetPr>
     <tabColor rgb="FF4F81BD"/>
   </sheetPr>
-  <dimension ref="A1:AMJ47"/>
+  <dimension ref="A1:AMJ50"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
@@ -745,12 +890,12 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
@@ -847,36 +992,36 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="27"/>
     </row>
     <row r="6" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -900,11 +1045,11 @@
       <c r="W6" s="6"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="6"/>
-      <c r="Z6" s="7"/>
+      <c r="Z6" s="28"/>
     </row>
     <row r="7" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
@@ -928,11 +1073,11 @@
       <c r="W7" s="8"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="8"/>
-      <c r="Z7" s="9"/>
+      <c r="Z7" s="29"/>
     </row>
     <row r="8" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="12"/>
@@ -956,11 +1101,11 @@
       <c r="W8" s="12"/>
       <c r="X8" s="13"/>
       <c r="Y8" s="12"/>
-      <c r="Z8" s="13"/>
+      <c r="Z8" s="30"/>
     </row>
     <row r="9" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
@@ -984,11 +1129,11 @@
       <c r="W9" s="8"/>
       <c r="X9" s="9"/>
       <c r="Y9" s="8"/>
-      <c r="Z9" s="9"/>
+      <c r="Z9" s="29"/>
     </row>
     <row r="10" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
       <c r="E10" s="12"/>
@@ -1012,11 +1157,11 @@
       <c r="W10" s="12"/>
       <c r="X10" s="13"/>
       <c r="Y10" s="12"/>
-      <c r="Z10" s="13"/>
+      <c r="Z10" s="30"/>
     </row>
     <row r="11" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
@@ -1040,11 +1185,11 @@
       <c r="W11" s="8"/>
       <c r="X11" s="9"/>
       <c r="Y11" s="8"/>
-      <c r="Z11" s="9"/>
+      <c r="Z11" s="29"/>
     </row>
     <row r="12" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="12"/>
@@ -1068,11 +1213,11 @@
       <c r="W12" s="12"/>
       <c r="X12" s="13"/>
       <c r="Y12" s="12"/>
-      <c r="Z12" s="13"/>
+      <c r="Z12" s="30"/>
     </row>
     <row r="13" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
       <c r="E13" s="8"/>
@@ -1096,11 +1241,11 @@
       <c r="W13" s="8"/>
       <c r="X13" s="9"/>
       <c r="Y13" s="8"/>
-      <c r="Z13" s="9"/>
+      <c r="Z13" s="29"/>
     </row>
     <row r="14" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
       <c r="E14" s="12"/>
@@ -1124,11 +1269,11 @@
       <c r="W14" s="12"/>
       <c r="X14" s="13"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="13"/>
+      <c r="Z14" s="30"/>
     </row>
     <row r="15" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
@@ -1152,11 +1297,11 @@
       <c r="W15" s="8"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="8"/>
-      <c r="Z15" s="9"/>
+      <c r="Z15" s="29"/>
     </row>
     <row r="16" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
       <c r="E16" s="12"/>
@@ -1180,11 +1325,11 @@
       <c r="W16" s="12"/>
       <c r="X16" s="13"/>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="13"/>
+      <c r="Z16" s="30"/>
     </row>
     <row r="17" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
@@ -1208,11 +1353,11 @@
       <c r="W17" s="8"/>
       <c r="X17" s="9"/>
       <c r="Y17" s="8"/>
-      <c r="Z17" s="9"/>
+      <c r="Z17" s="29"/>
     </row>
     <row r="18" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
       <c r="E18" s="12"/>
@@ -1236,11 +1381,11 @@
       <c r="W18" s="12"/>
       <c r="X18" s="13"/>
       <c r="Y18" s="12"/>
-      <c r="Z18" s="13"/>
+      <c r="Z18" s="30"/>
     </row>
     <row r="19" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
@@ -1264,11 +1409,11 @@
       <c r="W19" s="8"/>
       <c r="X19" s="9"/>
       <c r="Y19" s="8"/>
-      <c r="Z19" s="9"/>
+      <c r="Z19" s="29"/>
     </row>
     <row r="20" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
       <c r="E20" s="12"/>
@@ -1292,11 +1437,11 @@
       <c r="W20" s="12"/>
       <c r="X20" s="13"/>
       <c r="Y20" s="12"/>
-      <c r="Z20" s="13"/>
+      <c r="Z20" s="30"/>
     </row>
     <row r="21" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -1320,11 +1465,11 @@
       <c r="W21" s="8"/>
       <c r="X21" s="9"/>
       <c r="Y21" s="8"/>
-      <c r="Z21" s="9"/>
+      <c r="Z21" s="29"/>
     </row>
     <row r="22" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
       <c r="E22" s="12"/>
@@ -1348,11 +1493,11 @@
       <c r="W22" s="12"/>
       <c r="X22" s="13"/>
       <c r="Y22" s="12"/>
-      <c r="Z22" s="13"/>
+      <c r="Z22" s="30"/>
     </row>
     <row r="23" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -1376,11 +1521,11 @@
       <c r="W23" s="8"/>
       <c r="X23" s="9"/>
       <c r="Y23" s="8"/>
-      <c r="Z23" s="9"/>
+      <c r="Z23" s="29"/>
     </row>
     <row r="24" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
       <c r="E24" s="12"/>
@@ -1404,11 +1549,11 @@
       <c r="W24" s="12"/>
       <c r="X24" s="13"/>
       <c r="Y24" s="12"/>
-      <c r="Z24" s="13"/>
+      <c r="Z24" s="30"/>
     </row>
     <row r="25" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -1432,11 +1577,11 @@
       <c r="W25" s="8"/>
       <c r="X25" s="9"/>
       <c r="Y25" s="8"/>
-      <c r="Z25" s="9"/>
+      <c r="Z25" s="29"/>
     </row>
     <row r="26" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
       <c r="E26" s="12"/>
@@ -1460,11 +1605,11 @@
       <c r="W26" s="12"/>
       <c r="X26" s="13"/>
       <c r="Y26" s="12"/>
-      <c r="Z26" s="13"/>
+      <c r="Z26" s="30"/>
     </row>
     <row r="27" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
@@ -1488,11 +1633,11 @@
       <c r="W27" s="8"/>
       <c r="X27" s="9"/>
       <c r="Y27" s="8"/>
-      <c r="Z27" s="9"/>
+      <c r="Z27" s="29"/>
     </row>
     <row r="28" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
       <c r="E28" s="12"/>
@@ -1516,11 +1661,11 @@
       <c r="W28" s="12"/>
       <c r="X28" s="13"/>
       <c r="Y28" s="12"/>
-      <c r="Z28" s="13"/>
+      <c r="Z28" s="30"/>
     </row>
     <row r="29" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
@@ -1544,11 +1689,11 @@
       <c r="W29" s="8"/>
       <c r="X29" s="9"/>
       <c r="Y29" s="8"/>
-      <c r="Z29" s="9"/>
+      <c r="Z29" s="29"/>
     </row>
     <row r="30" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="12"/>
@@ -1572,11 +1717,11 @@
       <c r="W30" s="12"/>
       <c r="X30" s="13"/>
       <c r="Y30" s="12"/>
-      <c r="Z30" s="13"/>
+      <c r="Z30" s="30"/>
     </row>
     <row r="31" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="18"/>
       <c r="C31" s="8"/>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
@@ -1600,11 +1745,11 @@
       <c r="W31" s="8"/>
       <c r="X31" s="9"/>
       <c r="Y31" s="8"/>
-      <c r="Z31" s="9"/>
+      <c r="Z31" s="29"/>
     </row>
     <row r="32" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
       <c r="E32" s="12"/>
@@ -1628,11 +1773,11 @@
       <c r="W32" s="12"/>
       <c r="X32" s="13"/>
       <c r="Y32" s="12"/>
-      <c r="Z32" s="13"/>
+      <c r="Z32" s="30"/>
     </row>
     <row r="33" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="18"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
@@ -1656,11 +1801,11 @@
       <c r="W33" s="8"/>
       <c r="X33" s="9"/>
       <c r="Y33" s="8"/>
-      <c r="Z33" s="9"/>
+      <c r="Z33" s="29"/>
     </row>
     <row r="34" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
       <c r="E34" s="12"/>
@@ -1684,11 +1829,11 @@
       <c r="W34" s="12"/>
       <c r="X34" s="13"/>
       <c r="Y34" s="12"/>
-      <c r="Z34" s="13"/>
+      <c r="Z34" s="30"/>
     </row>
     <row r="35" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
@@ -1712,11 +1857,11 @@
       <c r="W35" s="8"/>
       <c r="X35" s="9"/>
       <c r="Y35" s="8"/>
-      <c r="Z35" s="9"/>
+      <c r="Z35" s="29"/>
     </row>
     <row r="36" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
       <c r="E36" s="12"/>
@@ -1740,11 +1885,11 @@
       <c r="W36" s="12"/>
       <c r="X36" s="13"/>
       <c r="Y36" s="12"/>
-      <c r="Z36" s="13"/>
+      <c r="Z36" s="30"/>
     </row>
     <row r="37" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="18"/>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
       <c r="E37" s="8"/>
@@ -1768,287 +1913,299 @@
       <c r="W37" s="8"/>
       <c r="X37" s="9"/>
       <c r="Y37" s="8"/>
-      <c r="Z37" s="9"/>
+      <c r="Z37" s="29"/>
     </row>
     <row r="38" spans="1:26" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
-      <c r="W38" s="18"/>
-      <c r="X38" s="18"/>
-      <c r="Y38" s="18"/>
-      <c r="Z38" s="18"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
+      <c r="Y38" s="16"/>
+      <c r="Z38" s="16"/>
     </row>
     <row r="39" spans="1:26" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
-      <c r="R39" s="23"/>
-      <c r="S39" s="23"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="23"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="23"/>
-      <c r="X39" s="23"/>
-      <c r="Y39" s="23"/>
-      <c r="Z39" s="23"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="21"/>
+      <c r="Z39" s="31"/>
     </row>
     <row r="40" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
-      <c r="R40" s="20"/>
-      <c r="S40" s="20"/>
-      <c r="T40" s="20"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="20"/>
-      <c r="W40" s="20"/>
-      <c r="X40" s="20"/>
-      <c r="Y40" s="20"/>
-      <c r="Z40" s="20"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="17"/>
+      <c r="W40" s="17"/>
+      <c r="X40" s="17"/>
+      <c r="Y40" s="17"/>
+      <c r="Z40" s="32"/>
     </row>
     <row r="41" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="19"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="18"/>
+      <c r="X41" s="18"/>
+      <c r="Y41" s="18"/>
+      <c r="Z41" s="33"/>
     </row>
     <row r="42" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
-      <c r="Q42" s="20"/>
-      <c r="R42" s="20"/>
-      <c r="S42" s="20"/>
-      <c r="T42" s="20"/>
-      <c r="U42" s="20"/>
-      <c r="V42" s="20"/>
-      <c r="W42" s="20"/>
-      <c r="X42" s="20"/>
-      <c r="Y42" s="20"/>
-      <c r="Z42" s="20"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
+      <c r="Z42" s="32"/>
     </row>
     <row r="43" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A43" s="21"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19"/>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19"/>
-      <c r="Y43" s="19"/>
-      <c r="Z43" s="19"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="18"/>
+      <c r="U43" s="18"/>
+      <c r="V43" s="18"/>
+      <c r="W43" s="18"/>
+      <c r="X43" s="18"/>
+      <c r="Y43" s="18"/>
+      <c r="Z43" s="33"/>
     </row>
     <row r="44" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
-      <c r="S44" s="20"/>
-      <c r="T44" s="20"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-      <c r="X44" s="20"/>
-      <c r="Y44" s="20"/>
-      <c r="Z44" s="20"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="17"/>
+      <c r="Y44" s="17"/>
+      <c r="Z44" s="32"/>
     </row>
     <row r="45" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A45" s="21"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="19"/>
-      <c r="Z45" s="19"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18"/>
+      <c r="U45" s="18"/>
+      <c r="V45" s="18"/>
+      <c r="W45" s="18"/>
+      <c r="X45" s="18"/>
+      <c r="Y45" s="18"/>
+      <c r="Z45" s="33"/>
     </row>
     <row r="46" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="20"/>
-      <c r="O46" s="20"/>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="20"/>
-      <c r="R46" s="20"/>
-      <c r="S46" s="20"/>
-      <c r="T46" s="20"/>
-      <c r="U46" s="20"/>
-      <c r="V46" s="20"/>
-      <c r="W46" s="20"/>
-      <c r="X46" s="20"/>
-      <c r="Y46" s="20"/>
-      <c r="Z46" s="20"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="17"/>
+      <c r="Y46" s="17"/>
+      <c r="Z46" s="32"/>
     </row>
     <row r="47" spans="1:26" ht="10.5" customHeight="1">
-      <c r="A47" s="21"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="19"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="19"/>
-      <c r="S47" s="19"/>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="19"/>
-      <c r="X47" s="19"/>
-      <c r="Y47" s="19"/>
-      <c r="Z47" s="19"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="18"/>
+      <c r="U47" s="18"/>
+      <c r="V47" s="18"/>
+      <c r="W47" s="18"/>
+      <c r="X47" s="18"/>
+      <c r="Y47" s="18"/>
+      <c r="Z47" s="33"/>
+    </row>
+    <row r="48" spans="1:26" ht="10.5" customHeight="1">
+      <c r="A48" s="41"/>
+      <c r="B48" s="41"/>
+    </row>
+    <row r="49" spans="1:2" ht="10.5" customHeight="1">
+      <c r="A49" s="41"/>
+      <c r="B49" s="41"/>
+    </row>
+    <row r="50" spans="1:2" ht="10.5" customHeight="1">
+      <c r="A50" s="41"/>
+      <c r="B50" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="163">
@@ -2148,6 +2305,9 @@
     <mergeCell ref="Q42:R42"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="U42:V42"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="O43:P43"/>
     <mergeCell ref="W42:X42"/>
     <mergeCell ref="Y42:Z42"/>
     <mergeCell ref="A43:B43"/>
@@ -2157,17 +2317,6 @@
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="W43:X43"/>
     <mergeCell ref="Y43:Z43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="O43:P43"/>
     <mergeCell ref="Q43:R43"/>
     <mergeCell ref="S43:T43"/>
     <mergeCell ref="U43:V43"/>
@@ -2181,6 +2330,14 @@
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="I45:J45"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O44:P44"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="E47:F47"/>
@@ -2205,6 +2362,7 @@
     <mergeCell ref="W47:X47"/>
     <mergeCell ref="Y47:Z47"/>
     <mergeCell ref="K47:L47"/>
+    <mergeCell ref="Y46:Z46"/>
     <mergeCell ref="M47:N47"/>
     <mergeCell ref="O47:P47"/>
     <mergeCell ref="Q47:R47"/>
@@ -2214,10 +2372,9 @@
     <mergeCell ref="S46:T46"/>
     <mergeCell ref="U46:V46"/>
     <mergeCell ref="W46:X46"/>
-    <mergeCell ref="Y46:Z46"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>